<commit_message>
AGG/Add estrous cycle processing to Shiny app
</commit_message>
<xml_diff>
--- a/data/excel-demo.xlsx
+++ b/data/excel-demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandagibson/Development/moenter-lab-r/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\percs\Documents\Development\moenter-lab-r\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDE0581-D63F-4349-862A-6A2C7082D5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2B9A67-57BC-4DA1-820F-D820BC4DDF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="1160" windowWidth="25440" windowHeight="14740" xr2:uid="{7E0C73D1-0F65-7841-9F2D-091518F52B09}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="6" xr2:uid="{7E0C73D1-0F65-7841-9F2D-091518F52B09}"/>
   </bookViews>
   <sheets>
     <sheet name="validation" sheetId="7" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="284">
   <si>
     <t>mouseID</t>
   </si>
@@ -765,69 +765,6 @@
     <t>AGD_P72</t>
   </si>
   <si>
-    <t>day1</t>
-  </si>
-  <si>
-    <t>day2</t>
-  </si>
-  <si>
-    <t>day3</t>
-  </si>
-  <si>
-    <t>day4</t>
-  </si>
-  <si>
-    <t>day5</t>
-  </si>
-  <si>
-    <t>day6</t>
-  </si>
-  <si>
-    <t>day7</t>
-  </si>
-  <si>
-    <t>day8</t>
-  </si>
-  <si>
-    <t>day9</t>
-  </si>
-  <si>
-    <t>day10</t>
-  </si>
-  <si>
-    <t>day11</t>
-  </si>
-  <si>
-    <t>day12</t>
-  </si>
-  <si>
-    <t>day13</t>
-  </si>
-  <si>
-    <t>day14</t>
-  </si>
-  <si>
-    <t>day15</t>
-  </si>
-  <si>
-    <t>day16</t>
-  </si>
-  <si>
-    <t>day17</t>
-  </si>
-  <si>
-    <t>day18</t>
-  </si>
-  <si>
-    <t>day19</t>
-  </si>
-  <si>
-    <t>day20</t>
-  </si>
-  <si>
-    <t>day21</t>
-  </si>
-  <si>
     <t>cycleNumber</t>
   </si>
   <si>
@@ -895,6 +832,75 @@
   </si>
   <si>
     <t>test3</t>
+  </si>
+  <si>
+    <t>cycleID</t>
+  </si>
+  <si>
+    <t>cycleStartDate</t>
+  </si>
+  <si>
+    <t>Day1</t>
+  </si>
+  <si>
+    <t>Day2</t>
+  </si>
+  <si>
+    <t>Day3</t>
+  </si>
+  <si>
+    <t>Day4</t>
+  </si>
+  <si>
+    <t>Day5</t>
+  </si>
+  <si>
+    <t>Day6</t>
+  </si>
+  <si>
+    <t>Day7</t>
+  </si>
+  <si>
+    <t>Day8</t>
+  </si>
+  <si>
+    <t>Day9</t>
+  </si>
+  <si>
+    <t>Day10</t>
+  </si>
+  <si>
+    <t>Day11</t>
+  </si>
+  <si>
+    <t>Day12</t>
+  </si>
+  <si>
+    <t>Day13</t>
+  </si>
+  <si>
+    <t>Day14</t>
+  </si>
+  <si>
+    <t>Day15</t>
+  </si>
+  <si>
+    <t>Day16</t>
+  </si>
+  <si>
+    <t>Day17</t>
+  </si>
+  <si>
+    <t>Day18</t>
+  </si>
+  <si>
+    <t>Day19</t>
+  </si>
+  <si>
+    <t>Day20</t>
+  </si>
+  <si>
+    <t>Day21</t>
   </si>
 </sst>
 </file>
@@ -903,8 +909,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="169" formatCode="0000000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -944,8 +950,8 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -953,19 +959,13 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -977,19 +977,25 @@
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0000000"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0000000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+      <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1009,13 +1015,13 @@
   <autoFilter ref="A1:J4" xr:uid="{C19D32EF-858A-9542-B09E-1B860703DEB6}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{2BD09072-F19D-B745-BE3D-925120B56AE1}" name="mouseID"/>
-    <tableColumn id="2" xr3:uid="{DBBAC3BE-34A1-2E48-B8D8-8B208D686E00}" name="cage" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{E8EBAB04-BDEC-EF4E-8879-5617D8190A00}" name="generation" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DBBAC3BE-34A1-2E48-B8D8-8B208D686E00}" name="cage" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E8EBAB04-BDEC-EF4E-8879-5617D8190A00}" name="generation" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{9A65C2A6-1FC4-6342-92BB-3C7531152163}" name="damID"/>
     <tableColumn id="5" xr3:uid="{D73EC5C9-9488-C746-80BB-A00DB8BEE0D1}" name="sireID"/>
     <tableColumn id="6" xr3:uid="{B6585CDB-CC84-1349-83A9-84115521032E}" name="specTreatment"/>
     <tableColumn id="7" xr3:uid="{F4A34ACA-EBC4-AB45-8724-FF7799320956}" name="treatment"/>
-    <tableColumn id="8" xr3:uid="{2E614C15-2700-E542-A4C4-FE10F6B0FBFF}" name="dateOfBirth" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{2E614C15-2700-E542-A4C4-FE10F6B0FBFF}" name="dateOfBirth" dataDxfId="10"/>
     <tableColumn id="9" xr3:uid="{FE5E4E7F-ABE4-8948-A048-4479593A80F0}" name="sex"/>
     <tableColumn id="10" xr3:uid="{DC288800-AB9E-3B4F-8698-92621EF5F704}" name="zygosity"/>
   </tableColumns>
@@ -1028,11 +1034,11 @@
   <autoFilter ref="A1:K4" xr:uid="{21B5469C-CBE7-B24D-9E03-E10DCDC459A8}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C6EFA388-C813-B449-AB75-14B2049A954C}" name="mouseID"/>
-    <tableColumn id="2" xr3:uid="{A6627528-F666-3048-AE13-D0D96D9A4DE1}" name="recordingDate" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{A6627528-F666-3048-AE13-D0D96D9A4DE1}" name="recordingDate" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{EE46710A-9A06-034D-87DA-A9C1A06C63BF}" name="savedPit"/>
     <tableColumn id="4" xr3:uid="{B9AF2EF2-4EFE-1D49-8EA7-1C755587FA68}" name="daylightSavings"/>
-    <tableColumn id="5" xr3:uid="{90B783E5-7F6C-8841-9508-42163B130436}" name="timeSac" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{F2EB051F-879E-3042-B84C-329FD108A572}" name="sac_hr" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{90B783E5-7F6C-8841-9508-42163B130436}" name="timeSac" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{F2EB051F-879E-3042-B84C-329FD108A572}" name="sac_hr" dataDxfId="7">
       <calculatedColumnFormula>IF(Table2[[#This Row],[daylightSavings]] = "Y", (Table2[[#This Row],[timeSac]] - 4/24) * 24, IF(Table2[[#This Row],[daylightSavings]] = "N", (Table2[[#This Row],[timeSac]]- 3/24)*24, ""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{52422692-60BC-E44F-BF65-8030018D5AC1}" name="whoSliced"/>
@@ -1052,12 +1058,12 @@
     <tableColumn id="1" xr3:uid="{13EE8625-C3D0-6D42-B8FD-A1CE95C5117C}" name="cellID"/>
     <tableColumn id="2" xr3:uid="{CB01B5A6-90FA-DA47-84DA-F5E66E864E7F}" name="mouseID"/>
     <tableColumn id="3" xr3:uid="{529DF6F5-04B5-5244-AD01-5EF0B2E629DB}" name="daylightSavings"/>
-    <tableColumn id="4" xr3:uid="{48328E1F-1D2E-2043-8522-ECC12A6613EA}" name="recordStart" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{F79F5373-DBE7-654A-9C74-4037D87244E0}" name="recordEnd" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{43BE574A-77B9-3B40-9825-E3DCE7A70D2D}" name="recordStart_hr" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{48328E1F-1D2E-2043-8522-ECC12A6613EA}" name="recordStart" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{F79F5373-DBE7-654A-9C74-4037D87244E0}" name="recordEnd" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{43BE574A-77B9-3B40-9825-E3DCE7A70D2D}" name="recordStart_hr" dataDxfId="4">
       <calculatedColumnFormula>IF(NOT(ISBLANK(Table3[[#This Row],[recordStart]])), IF(Table3[[#This Row],[daylightSavings]] = "Y", (Table3[[#This Row],[recordStart]] - 4/24) * 24, IF(Table3[[#This Row],[daylightSavings]] = "N", (Table3[[#This Row],[recordStart]]- 3/24)*24, "")), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1DC90344-9168-A54D-AFC1-F236A358ED19}" name="recordEnd_hr" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{1DC90344-9168-A54D-AFC1-F236A358ED19}" name="recordEnd_hr" dataDxfId="3">
       <calculatedColumnFormula>IF(NOT(ISBLANK(Table3[[#This Row],[recordEnd]])), IF(Table3[[#This Row],[daylightSavings]] = "Y", (Table3[[#This Row],[recordEnd]] - 4/24) * 24, IF(Table3[[#This Row],[daylightSavings]] = "N", (Table3[[#This Row],[recordEnd]]- 3/24)*24, "")), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{D176A103-C636-6247-8276-FCBFB914D727}" name="whoRecorded"/>
@@ -1275,31 +1281,33 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC15B1E3-5EB9-9A41-AFAF-3D20E11D0445}" name="Table6" displayName="Table6" ref="A1:V3" totalsRowShown="0">
-  <autoFilter ref="A1:V3" xr:uid="{038258B4-DFB8-BA43-9D86-8AA20442FE0A}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AC15B1E3-5EB9-9A41-AFAF-3D20E11D0445}" name="Table6" displayName="Table6" ref="A1:X3" totalsRowShown="0">
+  <autoFilter ref="A1:X3" xr:uid="{038258B4-DFB8-BA43-9D86-8AA20442FE0A}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{EDC5B09E-1E7D-D542-825F-E6C3920FBDD9}" name="mouseID"/>
-    <tableColumn id="2" xr3:uid="{DD7185D2-CC4E-4B4B-A35B-21131ADFD5D5}" name="day1"/>
-    <tableColumn id="3" xr3:uid="{C0DB3CF0-A5EE-E14D-A3CB-890535D24AF1}" name="day2"/>
-    <tableColumn id="4" xr3:uid="{4591C7C3-C247-7444-B631-F81493D1FF83}" name="day3"/>
-    <tableColumn id="5" xr3:uid="{7B784656-5BD4-D845-81C6-B0D21DD97770}" name="day4"/>
-    <tableColumn id="6" xr3:uid="{BD481F23-C370-6F40-86F0-0E052E658841}" name="day5"/>
-    <tableColumn id="7" xr3:uid="{2758C223-CC6C-6B4A-AD02-189CC16D23E9}" name="day6"/>
-    <tableColumn id="8" xr3:uid="{C18616EF-24F9-B744-919F-8FF02AAD1518}" name="day7"/>
-    <tableColumn id="9" xr3:uid="{3E7363B9-1C0D-F94B-86E2-F50956104F11}" name="day8"/>
-    <tableColumn id="10" xr3:uid="{DF0B1D04-1531-5343-9DC8-3BE959046735}" name="day9"/>
-    <tableColumn id="11" xr3:uid="{F8DFD5B0-160B-B54C-ACBE-659113086083}" name="day10"/>
-    <tableColumn id="12" xr3:uid="{DEBBBDF8-5CB1-AD4D-92F9-B228BC0C187A}" name="day11"/>
-    <tableColumn id="13" xr3:uid="{271B7C1C-7F3F-984E-AE72-BA2D2E812F5E}" name="day12"/>
-    <tableColumn id="14" xr3:uid="{4B0E64B7-315A-6F48-98CC-38143EB3B73D}" name="day13"/>
-    <tableColumn id="15" xr3:uid="{3CB76CE3-7019-C649-AA45-C0D1E01152EB}" name="day14"/>
-    <tableColumn id="16" xr3:uid="{7F6F439B-9B18-8645-AC05-7451A2F75F75}" name="day15"/>
-    <tableColumn id="17" xr3:uid="{8D34FED9-7B71-FC49-B71C-81F8EE283450}" name="day16"/>
-    <tableColumn id="18" xr3:uid="{81AD7CD3-533E-E144-B6C9-EB2EA2468A0F}" name="day17"/>
-    <tableColumn id="19" xr3:uid="{DAAF3F5C-355C-9242-B90A-0ABFB5D3DAAB}" name="day18"/>
-    <tableColumn id="20" xr3:uid="{450D152E-1874-9C47-8F18-FA2373918655}" name="day19"/>
-    <tableColumn id="21" xr3:uid="{9C5945BA-46D1-DC4C-879E-0DEA96F256EA}" name="day20"/>
-    <tableColumn id="22" xr3:uid="{5DA802B1-D1DA-7F4B-BCBC-C8956605A640}" name="day21"/>
+    <tableColumn id="24" xr3:uid="{A8EB749D-A023-4497-9E0C-236E09E78DAF}" name="cycleID"/>
+    <tableColumn id="23" xr3:uid="{88478318-B7C9-4796-A9D2-F760FEA9B2A0}" name="cycleStartDate"/>
+    <tableColumn id="2" xr3:uid="{DD7185D2-CC4E-4B4B-A35B-21131ADFD5D5}" name="Day1"/>
+    <tableColumn id="3" xr3:uid="{C0DB3CF0-A5EE-E14D-A3CB-890535D24AF1}" name="Day2"/>
+    <tableColumn id="4" xr3:uid="{4591C7C3-C247-7444-B631-F81493D1FF83}" name="Day3"/>
+    <tableColumn id="5" xr3:uid="{7B784656-5BD4-D845-81C6-B0D21DD97770}" name="Day4"/>
+    <tableColumn id="6" xr3:uid="{BD481F23-C370-6F40-86F0-0E052E658841}" name="Day5"/>
+    <tableColumn id="7" xr3:uid="{2758C223-CC6C-6B4A-AD02-189CC16D23E9}" name="Day6"/>
+    <tableColumn id="8" xr3:uid="{C18616EF-24F9-B744-919F-8FF02AAD1518}" name="Day7"/>
+    <tableColumn id="9" xr3:uid="{3E7363B9-1C0D-F94B-86E2-F50956104F11}" name="Day8"/>
+    <tableColumn id="10" xr3:uid="{DF0B1D04-1531-5343-9DC8-3BE959046735}" name="Day9"/>
+    <tableColumn id="11" xr3:uid="{F8DFD5B0-160B-B54C-ACBE-659113086083}" name="Day10"/>
+    <tableColumn id="12" xr3:uid="{DEBBBDF8-5CB1-AD4D-92F9-B228BC0C187A}" name="Day11"/>
+    <tableColumn id="13" xr3:uid="{271B7C1C-7F3F-984E-AE72-BA2D2E812F5E}" name="Day12"/>
+    <tableColumn id="14" xr3:uid="{4B0E64B7-315A-6F48-98CC-38143EB3B73D}" name="Day13"/>
+    <tableColumn id="15" xr3:uid="{3CB76CE3-7019-C649-AA45-C0D1E01152EB}" name="Day14"/>
+    <tableColumn id="16" xr3:uid="{7F6F439B-9B18-8645-AC05-7451A2F75F75}" name="Day15"/>
+    <tableColumn id="17" xr3:uid="{8D34FED9-7B71-FC49-B71C-81F8EE283450}" name="Day16"/>
+    <tableColumn id="18" xr3:uid="{81AD7CD3-533E-E144-B6C9-EB2EA2468A0F}" name="Day17"/>
+    <tableColumn id="19" xr3:uid="{DAAF3F5C-355C-9242-B90A-0ABFB5D3DAAB}" name="Day18"/>
+    <tableColumn id="20" xr3:uid="{450D152E-1874-9C47-8F18-FA2373918655}" name="Day19"/>
+    <tableColumn id="21" xr3:uid="{9C5945BA-46D1-DC4C-879E-0DEA96F256EA}" name="Day20"/>
+    <tableColumn id="22" xr3:uid="{5DA802B1-D1DA-7F4B-BCBC-C8956605A640}" name="Day21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1645,13 +1653,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E7E6FB-2534-F647-ABDC-4D87D50A6DA8}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>211</v>
       </c>
@@ -1665,10 +1673,10 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1685,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>215</v>
       </c>
@@ -1713,7 +1721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>222</v>
       </c>
@@ -1731,15 +1739,15 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.296875" customWidth="1"/>
+    <col min="6" max="6" width="15.796875" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1771,9 +1779,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -1782,30 +1790,30 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="F2" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="G2" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="H2" s="2">
         <v>44197</v>
       </c>
       <c r="I2" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="J2" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1814,30 +1822,30 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="E3" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="F3" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="G3" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="H3" s="2">
         <v>44197</v>
       </c>
       <c r="I3" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="J3" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1862,18 +1870,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" customWidth="1"/>
+    <col min="7" max="7" width="11.796875" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" customWidth="1"/>
+    <col min="9" max="9" width="13.69921875" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1890,7 +1898,7 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -1908,9 +1916,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2">
         <v>44256</v>
@@ -1929,7 +1937,7 @@
         <v>10.000000000000002</v>
       </c>
       <c r="G2" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="H2" t="s">
         <v>219</v>
@@ -1944,9 +1952,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="B3" s="2">
         <v>44287</v>
@@ -1965,7 +1973,7 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
         <v>220</v>
@@ -1980,9 +1988,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="B4" s="2">
         <v>44215</v>
@@ -2017,16 +2025,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" customWidth="1"/>
+    <col min="6" max="8" width="14.69921875" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2043,10 +2051,10 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="G1" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="H1" t="s">
         <v>22</v>
@@ -2064,15 +2072,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1">
         <v>0.66666666666666663</v>
@@ -2089,7 +2097,7 @@
         <v>13.000000000000002</v>
       </c>
       <c r="H2" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="I2" t="s">
         <v>215</v>
@@ -2125,14 +2133,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2146,9 +2154,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2176,14 +2184,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="11" width="11.1640625" customWidth="1"/>
-    <col min="12" max="101" width="12.1640625" customWidth="1"/>
-    <col min="102" max="182" width="13.1640625" customWidth="1"/>
+    <col min="2" max="11" width="11.19921875" customWidth="1"/>
+    <col min="12" max="101" width="12.19921875" customWidth="1"/>
+    <col min="102" max="182" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:182" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:182" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -2731,9 +2739,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:182" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:182" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2759,138 +2767,138 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82174D8D-9F0C-6A48-A8E8-B1CEEC6E2F35}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="D1" t="s">
-        <v>240</v>
+        <v>263</v>
       </c>
       <c r="E1" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="F1" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
       <c r="G1" t="s">
-        <v>243</v>
+        <v>266</v>
       </c>
       <c r="H1" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="I1" t="s">
-        <v>245</v>
+        <v>268</v>
       </c>
       <c r="J1" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="K1" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="L1" t="s">
-        <v>248</v>
+        <v>271</v>
       </c>
       <c r="M1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="N1" t="s">
+        <v>273</v>
+      </c>
+      <c r="O1" t="s">
+        <v>274</v>
+      </c>
+      <c r="P1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R1" t="s">
+        <v>277</v>
+      </c>
+      <c r="S1" t="s">
+        <v>278</v>
+      </c>
+      <c r="T1" t="s">
+        <v>279</v>
+      </c>
+      <c r="U1" t="s">
+        <v>280</v>
+      </c>
+      <c r="V1" t="s">
+        <v>281</v>
+      </c>
+      <c r="W1" t="s">
+        <v>282</v>
+      </c>
+      <c r="X1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>250</v>
       </c>
-      <c r="O1" t="s">
-        <v>251</v>
-      </c>
-      <c r="P1" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>253</v>
-      </c>
-      <c r="R1" t="s">
-        <v>254</v>
-      </c>
-      <c r="S1" t="s">
-        <v>255</v>
-      </c>
-      <c r="T1" t="s">
-        <v>256</v>
-      </c>
-      <c r="U1" t="s">
-        <v>257</v>
-      </c>
-      <c r="V1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>3</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
       </c>
       <c r="M2">
         <v>2</v>
       </c>
       <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+        <v>255</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2947,13 +2955,19 @@
         <v>2</v>
       </c>
       <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:V3" xr:uid="{00E8F842-E4D3-984A-8178-A77D161C465C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:X3" xr:uid="{00E8F842-E4D3-984A-8178-A77D161C465C}">
       <formula1>cycleNumber</formula1>
     </dataValidation>
   </dataValidations>
@@ -2972,42 +2986,42 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.69921875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.69921875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C1" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="E1" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="F1" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="G1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -3044,19 +3058,19 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.296875" customWidth="1"/>
+    <col min="5" max="5" width="12.296875" customWidth="1"/>
+    <col min="6" max="6" width="13.796875" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.1640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="16" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.69921875" customWidth="1"/>
+    <col min="9" max="9" width="19.19921875" customWidth="1"/>
+    <col min="10" max="10" width="17.796875" customWidth="1"/>
+    <col min="11" max="16" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3106,9 +3120,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2">
         <v>44281</v>

</xml_diff>